<commit_message>
trying to add codes to profit for df2
</commit_message>
<xml_diff>
--- a/questions/successful_tour_looks_like.xlsx
+++ b/questions/successful_tour_looks_like.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,16 +501,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>4.350544765513974</v>
+        <v>4.351172152498224</v>
       </c>
       <c r="D3" t="n">
-        <v>4222</v>
+        <v>4223</v>
       </c>
       <c r="E3" t="n">
-        <v>2.178588346755092</v>
+        <v>2.178309258820744</v>
       </c>
       <c r="F3" t="n">
-        <v>307776.75</v>
+        <v>307807.89</v>
       </c>
     </row>
     <row r="4">
@@ -573,16 +573,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>4.220858895705521</v>
+        <v>4.215568862275449</v>
       </c>
       <c r="D6" t="n">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="E6" t="n">
-        <v>1.45398773006135</v>
+        <v>1.491017964071856</v>
       </c>
       <c r="F6" t="n">
-        <v>7224.5</v>
+        <v>7348.5</v>
       </c>
     </row>
     <row r="7">
@@ -593,20 +593,20 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>July</t>
+          <t>June</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>4.308291991495393</v>
+        <v>4.164274924471299</v>
       </c>
       <c r="D7" t="n">
-        <v>2822</v>
+        <v>2648</v>
       </c>
       <c r="E7" t="n">
-        <v>1.978029766123317</v>
+        <v>1.95392749244713</v>
       </c>
       <c r="F7" t="n">
-        <v>203700.31</v>
+        <v>182864</v>
       </c>
     </row>
     <row r="8">
@@ -617,20 +617,20 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>June</t>
+          <t>March</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>4.164461247637051</v>
+        <v>5.923076923076923</v>
       </c>
       <c r="D8" t="n">
-        <v>2645</v>
+        <v>572</v>
       </c>
       <c r="E8" t="n">
-        <v>1.952741020793951</v>
+        <v>1.694055944055944</v>
       </c>
       <c r="F8" t="n">
-        <v>182771</v>
+        <v>34128</v>
       </c>
     </row>
     <row r="9">
@@ -641,20 +641,20 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>March</t>
+          <t>May</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>5.948853615520282</v>
+        <v>4.27736890524379</v>
       </c>
       <c r="D9" t="n">
-        <v>567</v>
+        <v>2174</v>
       </c>
       <c r="E9" t="n">
-        <v>1.700176366843033</v>
+        <v>2.10395584176633</v>
       </c>
       <c r="F9" t="n">
-        <v>33973</v>
+        <v>150305.46</v>
       </c>
     </row>
     <row r="10">
@@ -665,20 +665,20 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>May</t>
+          <t>November</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>4.27736890524379</v>
+        <v>4.117021276595745</v>
       </c>
       <c r="D10" t="n">
-        <v>2174</v>
+        <v>282</v>
       </c>
       <c r="E10" t="n">
-        <v>2.10395584176633</v>
+        <v>1.439716312056738</v>
       </c>
       <c r="F10" t="n">
-        <v>150305.46</v>
+        <v>12941.32</v>
       </c>
     </row>
     <row r="11">
@@ -689,20 +689,20 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>November</t>
+          <t>October</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>4.117021276595745</v>
+        <v>4.22294776119403</v>
       </c>
       <c r="D11" t="n">
-        <v>282</v>
+        <v>1072</v>
       </c>
       <c r="E11" t="n">
-        <v>1.439716312056738</v>
+        <v>1.800373134328358</v>
       </c>
       <c r="F11" t="n">
-        <v>12941.32</v>
+        <v>72117.32000000001</v>
       </c>
     </row>
     <row r="12">
@@ -713,44 +713,44 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>October</t>
+          <t>September</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>4.223155929038282</v>
+        <v>4.158210947930574</v>
       </c>
       <c r="D12" t="n">
-        <v>1071</v>
+        <v>1498</v>
       </c>
       <c r="E12" t="n">
-        <v>1.799253034547152</v>
+        <v>2.068758344459279</v>
       </c>
       <c r="F12" t="n">
-        <v>72086.32000000001</v>
+        <v>102478.57</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Greece</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>September</t>
+          <t>April</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>4.158210947930574</v>
+        <v>4.205128205128205</v>
       </c>
       <c r="D13" t="n">
-        <v>1498</v>
+        <v>312</v>
       </c>
       <c r="E13" t="n">
-        <v>2.068758344459279</v>
+        <v>1.375</v>
       </c>
       <c r="F13" t="n">
-        <v>102478.57</v>
+        <v>28415</v>
       </c>
     </row>
     <row r="14">
@@ -761,20 +761,20 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>April</t>
+          <t>August</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>4.205128205128205</v>
+        <v>3</v>
       </c>
       <c r="D14" t="n">
-        <v>312</v>
+        <v>40</v>
       </c>
       <c r="E14" t="n">
         <v>1.375</v>
       </c>
       <c r="F14" t="n">
-        <v>28415</v>
+        <v>2245</v>
       </c>
     </row>
     <row r="15">
@@ -785,20 +785,20 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>August</t>
+          <t>February</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>3</v>
+        <v>3.461538461538462</v>
       </c>
       <c r="D15" t="n">
-        <v>40</v>
+        <v>104</v>
       </c>
       <c r="E15" t="n">
         <v>1.375</v>
       </c>
       <c r="F15" t="n">
-        <v>2245</v>
+        <v>7229</v>
       </c>
     </row>
     <row r="16">
@@ -809,20 +809,20 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>February</t>
+          <t>January</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3.461538461538462</v>
+        <v>4</v>
       </c>
       <c r="D16" t="n">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="E16" t="n">
         <v>1.375</v>
       </c>
       <c r="F16" t="n">
-        <v>7229</v>
+        <v>10215</v>
       </c>
     </row>
     <row r="17">
@@ -833,20 +833,20 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>January</t>
+          <t>June</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>4</v>
+        <v>3.777777777777778</v>
       </c>
       <c r="D17" t="n">
-        <v>120</v>
+        <v>72</v>
       </c>
       <c r="E17" t="n">
         <v>1.375</v>
       </c>
       <c r="F17" t="n">
-        <v>10215</v>
+        <v>5665</v>
       </c>
     </row>
     <row r="18">
@@ -857,20 +857,20 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>July</t>
+          <t>March</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>3.6</v>
+        <v>6</v>
       </c>
       <c r="D18" t="n">
-        <v>40</v>
+        <v>88</v>
       </c>
       <c r="E18" t="n">
         <v>1.375</v>
       </c>
       <c r="F18" t="n">
-        <v>2941</v>
+        <v>12595</v>
       </c>
     </row>
     <row r="19">
@@ -881,20 +881,20 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>June</t>
+          <t>May</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>3.777777777777778</v>
+        <v>5.272727272727272</v>
       </c>
       <c r="D19" t="n">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="E19" t="n">
         <v>1.375</v>
       </c>
       <c r="F19" t="n">
-        <v>5665</v>
+        <v>10739</v>
       </c>
     </row>
     <row r="20">
@@ -905,20 +905,20 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>March</t>
+          <t>November</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>6</v>
+        <v>4.557692307692307</v>
       </c>
       <c r="D20" t="n">
-        <v>88</v>
+        <v>52</v>
       </c>
       <c r="E20" t="n">
-        <v>1.375</v>
+        <v>1.288461538461539</v>
       </c>
       <c r="F20" t="n">
-        <v>12595</v>
+        <v>4614</v>
       </c>
     </row>
     <row r="21">
@@ -929,20 +929,20 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>May</t>
+          <t>October</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>5.272727272727272</v>
+        <v>3.844660194174757</v>
       </c>
       <c r="D21" t="n">
-        <v>88</v>
+        <v>206</v>
       </c>
       <c r="E21" t="n">
-        <v>1.375</v>
+        <v>1.276699029126214</v>
       </c>
       <c r="F21" t="n">
-        <v>10739</v>
+        <v>13953</v>
       </c>
     </row>
     <row r="22">
@@ -953,68 +953,68 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>November</t>
+          <t>September</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>4.557692307692307</v>
+        <v>3.75</v>
       </c>
       <c r="D22" t="n">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="E22" t="n">
-        <v>1.288461538461539</v>
+        <v>1.375</v>
       </c>
       <c r="F22" t="n">
-        <v>4614</v>
+        <v>4161.12</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>Portugal</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>October</t>
+          <t>April</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>3.844660194174757</v>
+        <v>4.089038385437277</v>
       </c>
       <c r="D23" t="n">
-        <v>206</v>
+        <v>2527</v>
       </c>
       <c r="E23" t="n">
-        <v>1.276699029126214</v>
+        <v>1.6398891966759</v>
       </c>
       <c r="F23" t="n">
-        <v>13953</v>
+        <v>173967.5</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>Portugal</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>September</t>
+          <t>August</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>3.75</v>
+        <v>4.164769647696477</v>
       </c>
       <c r="D24" t="n">
-        <v>64</v>
+        <v>1845</v>
       </c>
       <c r="E24" t="n">
-        <v>1.375</v>
+        <v>1.38319783197832</v>
       </c>
       <c r="F24" t="n">
-        <v>4161.12</v>
+        <v>119299.68</v>
       </c>
     </row>
     <row r="25">
@@ -1025,20 +1025,20 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>April</t>
+          <t>December</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>4.089038385437277</v>
+        <v>4.112244897959184</v>
       </c>
       <c r="D25" t="n">
-        <v>2527</v>
+        <v>196</v>
       </c>
       <c r="E25" t="n">
-        <v>1.6398891966759</v>
+        <v>1.173469387755102</v>
       </c>
       <c r="F25" t="n">
-        <v>173967.5</v>
+        <v>10991.2</v>
       </c>
     </row>
     <row r="26">
@@ -1049,20 +1049,20 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>August</t>
+          <t>February</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>4.164769647696477</v>
+        <v>3.720812182741117</v>
       </c>
       <c r="D26" t="n">
-        <v>1845</v>
+        <v>197</v>
       </c>
       <c r="E26" t="n">
-        <v>1.38319783197832</v>
+        <v>1.467005076142132</v>
       </c>
       <c r="F26" t="n">
-        <v>119299.68</v>
+        <v>10560.04</v>
       </c>
     </row>
     <row r="27">
@@ -1073,20 +1073,20 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>December</t>
+          <t>January</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>4.112244897959184</v>
+        <v>3.961832061068702</v>
       </c>
       <c r="D27" t="n">
-        <v>196</v>
+        <v>131</v>
       </c>
       <c r="E27" t="n">
-        <v>1.173469387755102</v>
+        <v>1.595419847328244</v>
       </c>
       <c r="F27" t="n">
-        <v>10991.2</v>
+        <v>7772</v>
       </c>
     </row>
     <row r="28">
@@ -1097,20 +1097,20 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>February</t>
+          <t>June</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>3.720812182741117</v>
+        <v>4.231991525423729</v>
       </c>
       <c r="D28" t="n">
-        <v>197</v>
+        <v>1888</v>
       </c>
       <c r="E28" t="n">
-        <v>1.467005076142132</v>
+        <v>1.621822033898305</v>
       </c>
       <c r="F28" t="n">
-        <v>10560.04</v>
+        <v>136740.7</v>
       </c>
     </row>
     <row r="29">
@@ -1121,20 +1121,20 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>January</t>
+          <t>March</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>3.961832061068702</v>
+        <v>3.949392712550607</v>
       </c>
       <c r="D29" t="n">
-        <v>131</v>
+        <v>494</v>
       </c>
       <c r="E29" t="n">
-        <v>1.595419847328244</v>
+        <v>1.629554655870445</v>
       </c>
       <c r="F29" t="n">
-        <v>7772</v>
+        <v>33100.7</v>
       </c>
     </row>
     <row r="30">
@@ -1145,20 +1145,20 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>July</t>
+          <t>May</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>4.372266401590458</v>
+        <v>4.262116316639742</v>
       </c>
       <c r="D30" t="n">
-        <v>2012</v>
+        <v>2476</v>
       </c>
       <c r="E30" t="n">
-        <v>1.541252485089463</v>
+        <v>1.644184168012924</v>
       </c>
       <c r="F30" t="n">
-        <v>142488.2</v>
+        <v>179698</v>
       </c>
     </row>
     <row r="31">
@@ -1169,20 +1169,20 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>June</t>
+          <t>November</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>4.231991525423729</v>
+        <v>4.085106382978723</v>
       </c>
       <c r="D31" t="n">
-        <v>1888</v>
+        <v>329</v>
       </c>
       <c r="E31" t="n">
-        <v>1.621822033898305</v>
+        <v>1.288753799392097</v>
       </c>
       <c r="F31" t="n">
-        <v>136740.7</v>
+        <v>20496.6</v>
       </c>
     </row>
     <row r="32">
@@ -1193,20 +1193,20 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>March</t>
+          <t>October</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>3.949392712550607</v>
+        <v>3.954545454545455</v>
       </c>
       <c r="D32" t="n">
-        <v>494</v>
+        <v>1100</v>
       </c>
       <c r="E32" t="n">
-        <v>1.629554655870445</v>
+        <v>1.493636363636364</v>
       </c>
       <c r="F32" t="n">
-        <v>33100.7</v>
+        <v>70794.60000000001</v>
       </c>
     </row>
     <row r="33">
@@ -1217,92 +1217,92 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>May</t>
+          <t>September</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>4.262116316639742</v>
+        <v>3.888774459320288</v>
       </c>
       <c r="D33" t="n">
-        <v>2476</v>
+        <v>971</v>
       </c>
       <c r="E33" t="n">
-        <v>1.644184168012924</v>
+        <v>1.440782698249228</v>
       </c>
       <c r="F33" t="n">
-        <v>179698</v>
+        <v>58716</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Portugal</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>November</t>
+          <t>April</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>4.085106382978723</v>
+        <v>4.551724137931035</v>
       </c>
       <c r="D34" t="n">
-        <v>329</v>
+        <v>87</v>
       </c>
       <c r="E34" t="n">
-        <v>1.288753799392097</v>
+        <v>1.172413793103448</v>
       </c>
       <c r="F34" t="n">
-        <v>20496.6</v>
+        <v>7231.46</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Portugal</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>October</t>
+          <t>August</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>3.954545454545455</v>
+        <v>4.133928571428571</v>
       </c>
       <c r="D35" t="n">
-        <v>1100</v>
+        <v>224</v>
       </c>
       <c r="E35" t="n">
-        <v>1.493636363636364</v>
+        <v>1.209821428571429</v>
       </c>
       <c r="F35" t="n">
-        <v>70794.60000000001</v>
+        <v>18747.7</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Portugal</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>September</t>
+          <t>December</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>3.888774459320288</v>
+        <v>3.777777777777778</v>
       </c>
       <c r="D36" t="n">
-        <v>971</v>
+        <v>45</v>
       </c>
       <c r="E36" t="n">
-        <v>1.440782698249228</v>
+        <v>1.155555555555555</v>
       </c>
       <c r="F36" t="n">
-        <v>58716</v>
+        <v>2890</v>
       </c>
     </row>
     <row r="37">
@@ -1313,20 +1313,20 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>April</t>
+          <t>June</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>4.551724137931035</v>
+        <v>3.567901234567901</v>
       </c>
       <c r="D37" t="n">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E37" t="n">
-        <v>1.172413793103448</v>
+        <v>1.185185185185185</v>
       </c>
       <c r="F37" t="n">
-        <v>7231.46</v>
+        <v>5520.82</v>
       </c>
     </row>
     <row r="38">
@@ -1337,20 +1337,20 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>August</t>
+          <t>May</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>4.133928571428571</v>
+        <v>3.777777777777778</v>
       </c>
       <c r="D38" t="n">
-        <v>224</v>
+        <v>81</v>
       </c>
       <c r="E38" t="n">
-        <v>1.209821428571429</v>
+        <v>1.209876543209877</v>
       </c>
       <c r="F38" t="n">
-        <v>18747.7</v>
+        <v>5793.78</v>
       </c>
     </row>
     <row r="39">
@@ -1361,20 +1361,20 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>December</t>
+          <t>November</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>3.777777777777778</v>
+        <v>4.212355212355212</v>
       </c>
       <c r="D39" t="n">
-        <v>45</v>
+        <v>259</v>
       </c>
       <c r="E39" t="n">
-        <v>1.155555555555555</v>
+        <v>1.173745173745174</v>
       </c>
       <c r="F39" t="n">
-        <v>2890</v>
+        <v>19154.92</v>
       </c>
     </row>
     <row r="40">
@@ -1385,20 +1385,20 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>July</t>
+          <t>October</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>4.304347826086956</v>
+        <v>3.787446504992867</v>
       </c>
       <c r="D40" t="n">
-        <v>115</v>
+        <v>701</v>
       </c>
       <c r="E40" t="n">
-        <v>1.2</v>
+        <v>1.156918687589158</v>
       </c>
       <c r="F40" t="n">
-        <v>10617</v>
+        <v>47079.84</v>
       </c>
     </row>
     <row r="41">
@@ -1409,163 +1409,67 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>June</t>
+          <t>September</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>3.567901234567901</v>
+        <v>3.989690721649485</v>
       </c>
       <c r="D41" t="n">
-        <v>81</v>
+        <v>194</v>
       </c>
       <c r="E41" t="n">
-        <v>1.185185185185185</v>
+        <v>1.164948453608248</v>
       </c>
       <c r="F41" t="n">
-        <v>5520.82</v>
+        <v>13759.46</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>May</t>
+          <t>October</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>3.777777777777778</v>
+        <v>2.311111111111111</v>
       </c>
       <c r="D42" t="n">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="E42" t="n">
-        <v>1.209876543209877</v>
+        <v>1</v>
       </c>
       <c r="F42" t="n">
-        <v>5793.78</v>
+        <v>2038</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>November</t>
+          <t>September</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>4.212355212355212</v>
+        <v>2.64</v>
       </c>
       <c r="D43" t="n">
-        <v>259</v>
+        <v>50</v>
       </c>
       <c r="E43" t="n">
-        <v>1.173745173745174</v>
+        <v>1</v>
       </c>
       <c r="F43" t="n">
-        <v>19154.92</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>Spain</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>October</t>
-        </is>
-      </c>
-      <c r="C44" t="n">
-        <v>3.787446504992867</v>
-      </c>
-      <c r="D44" t="n">
-        <v>701</v>
-      </c>
-      <c r="E44" t="n">
-        <v>1.156918687589158</v>
-      </c>
-      <c r="F44" t="n">
-        <v>47079.84</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>Spain</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>September</t>
-        </is>
-      </c>
-      <c r="C45" t="n">
-        <v>3.989690721649485</v>
-      </c>
-      <c r="D45" t="n">
-        <v>194</v>
-      </c>
-      <c r="E45" t="n">
-        <v>1.164948453608248</v>
-      </c>
-      <c r="F45" t="n">
-        <v>13759.46</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>Turkey</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>October</t>
-        </is>
-      </c>
-      <c r="C46" t="n">
-        <v>2.311111111111111</v>
-      </c>
-      <c r="D46" t="n">
-        <v>45</v>
-      </c>
-      <c r="E46" t="n">
-        <v>1</v>
-      </c>
-      <c r="F46" t="n">
-        <v>2038</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>Turkey</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>September</t>
-        </is>
-      </c>
-      <c r="C47" t="n">
-        <v>2.64</v>
-      </c>
-      <c r="D47" t="n">
-        <v>50</v>
-      </c>
-      <c r="E47" t="n">
-        <v>1</v>
-      </c>
-      <c r="F47" t="n">
         <v>2710</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added travel and booking days, and booking hours
</commit_message>
<xml_diff>
--- a/questions/successful_tour_looks_like.xlsx
+++ b/questions/successful_tour_looks_like.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
added more to functions
</commit_message>
<xml_diff>
--- a/questions/successful_tour_looks_like.xlsx
+++ b/questions/successful_tour_looks_like.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +464,21 @@
           <t>Total_profit</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Top_3_travel_days</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Average_Money_Spent</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>most_common_languages</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -473,20 +488,33 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>April</t>
+          <t>August</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>4.197818542389688</v>
+        <v>4.351172152498224</v>
       </c>
       <c r="D2" t="n">
-        <v>2017</v>
+        <v>4223</v>
       </c>
       <c r="E2" t="n">
-        <v>2.119484382746653</v>
+        <v>2.178309258820744</v>
       </c>
       <c r="F2" t="n">
-        <v>132476.5</v>
+        <v>307807.89</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>[('Wednesday', 810), ('Thursday', 635), ('Sunday', 631)]</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>104.7646530902202</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>['English']</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -497,68 +525,107 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>August</t>
+          <t>June</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>4.351172152498224</v>
+        <v>4.164274924471299</v>
       </c>
       <c r="D3" t="n">
-        <v>4223</v>
+        <v>2648</v>
       </c>
       <c r="E3" t="n">
-        <v>2.178309258820744</v>
+        <v>1.95392749244713</v>
       </c>
       <c r="F3" t="n">
-        <v>307807.89</v>
+        <v>182864</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>[('Friday', 483), ('Thursday', 482), ('Monday', 430)]</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>97.91842900302115</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>['English']</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Greece</t>
+          <t>Portugal</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>December</t>
+          <t>May</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>4.520833333333333</v>
+        <v>4.262116316639742</v>
       </c>
       <c r="D4" t="n">
-        <v>48</v>
+        <v>2476</v>
       </c>
       <c r="E4" t="n">
-        <v>1.208333333333333</v>
+        <v>1.644184168012924</v>
       </c>
       <c r="F4" t="n">
-        <v>2150.8</v>
+        <v>179698</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>[('Monday', 414), ('Thursday', 386), ('Friday', 383)]</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>98.8620759289176</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>['English']</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Greece</t>
+          <t>Portugal</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>February</t>
+          <t>April</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>7.565749235474006</v>
+        <v>4.089038385437277</v>
       </c>
       <c r="D5" t="n">
-        <v>327</v>
+        <v>2527</v>
       </c>
       <c r="E5" t="n">
-        <v>1.749235474006116</v>
+        <v>1.6398891966759</v>
       </c>
       <c r="F5" t="n">
-        <v>26937</v>
+        <v>173967.5</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>[('Monday', 552), ('Sunday', 455), ('Friday', 363)]</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>95.22041946972695</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>['English']</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -569,26 +636,39 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>January</t>
+          <t>May</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>4.215568862275449</v>
+        <v>4.27736890524379</v>
       </c>
       <c r="D6" t="n">
-        <v>167</v>
+        <v>2174</v>
       </c>
       <c r="E6" t="n">
-        <v>1.491017964071856</v>
+        <v>2.10395584176633</v>
       </c>
       <c r="F6" t="n">
-        <v>7348.5</v>
+        <v>150305.46</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>[('Wednesday', 440), ('Tuesday', 371), ('Friday', 334)]</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>99.91595216191352</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>['English']</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Greece</t>
+          <t>Portugal</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -597,16 +677,29 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>4.164274924471299</v>
+        <v>4.231991525423729</v>
       </c>
       <c r="D7" t="n">
-        <v>2648</v>
+        <v>1888</v>
       </c>
       <c r="E7" t="n">
-        <v>1.95392749244713</v>
+        <v>1.621822033898305</v>
       </c>
       <c r="F7" t="n">
-        <v>182864</v>
+        <v>136740.7</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>[('Monday', 344), ('Friday', 318), ('Thursday', 286)]</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>98.68495762711865</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>['English']</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -617,44 +710,70 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>March</t>
+          <t>April</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>5.923076923076923</v>
+        <v>4.197818542389688</v>
       </c>
       <c r="D8" t="n">
-        <v>572</v>
+        <v>2017</v>
       </c>
       <c r="E8" t="n">
-        <v>1.694055944055944</v>
+        <v>2.119484382746653</v>
       </c>
       <c r="F8" t="n">
-        <v>34128</v>
+        <v>132476.5</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>[('Saturday', 423), ('Friday', 312), ('Sunday', 302)]</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>96.90059494298463</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>['English']</t>
+        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Greece</t>
+          <t>Portugal</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>May</t>
+          <t>August</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>4.27736890524379</v>
+        <v>4.164769647696477</v>
       </c>
       <c r="D9" t="n">
-        <v>2174</v>
+        <v>1845</v>
       </c>
       <c r="E9" t="n">
-        <v>2.10395584176633</v>
+        <v>1.38319783197832</v>
       </c>
       <c r="F9" t="n">
-        <v>150305.46</v>
+        <v>119299.68</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>[('Thursday', 377), ('Tuesday', 335), ('Wednesday', 313)]</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>87.53344173441735</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>['English']</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -665,20 +784,33 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>November</t>
+          <t>September</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>4.117021276595745</v>
+        <v>4.158210947930574</v>
       </c>
       <c r="D10" t="n">
-        <v>282</v>
+        <v>1498</v>
       </c>
       <c r="E10" t="n">
-        <v>1.439716312056738</v>
+        <v>2.068758344459279</v>
       </c>
       <c r="F10" t="n">
-        <v>12941.32</v>
+        <v>102478.57</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>[('Friday', 308), ('Saturday', 255), ('Thursday', 233)]</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>99.51302403204274</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>['English']</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -704,125 +836,203 @@
       <c r="F11" t="n">
         <v>72117.32000000001</v>
       </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>[('Monday', 236), ('Tuesday', 202), ('Wednesday', 173)]</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>93.98205223880596</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>['English']</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Greece</t>
+          <t>Portugal</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>September</t>
+          <t>October</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>4.158210947930574</v>
+        <v>3.954545454545455</v>
       </c>
       <c r="D12" t="n">
-        <v>1498</v>
+        <v>1100</v>
       </c>
       <c r="E12" t="n">
-        <v>2.068758344459279</v>
+        <v>1.493636363636364</v>
       </c>
       <c r="F12" t="n">
-        <v>102478.57</v>
+        <v>70794.60000000001</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>[('Saturday', 197), ('Monday', 193), ('Wednesday', 184)]</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>89.30600000000001</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>['English']</t>
+        </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>Portugal</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>April</t>
+          <t>September</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>4.205128205128205</v>
+        <v>3.888774459320288</v>
       </c>
       <c r="D13" t="n">
-        <v>312</v>
+        <v>971</v>
       </c>
       <c r="E13" t="n">
-        <v>1.375</v>
+        <v>1.440782698249228</v>
       </c>
       <c r="F13" t="n">
-        <v>28415</v>
+        <v>58716</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>[('Saturday', 166), ('Monday', 157), ('Friday', 152)]</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>84.68898043254377</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>['English']</t>
+        </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>August</t>
+          <t>October</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>3</v>
+        <v>3.787446504992867</v>
       </c>
       <c r="D14" t="n">
-        <v>40</v>
+        <v>701</v>
       </c>
       <c r="E14" t="n">
-        <v>1.375</v>
+        <v>1.156918687589158</v>
       </c>
       <c r="F14" t="n">
-        <v>2245</v>
+        <v>47079.84</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>[('Monday', 128), ('Tuesday', 114), ('Sunday', 106)]</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>91.57888730385164</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>['English']</t>
+        </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>Greece</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>February</t>
+          <t>March</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>3.461538461538462</v>
+        <v>5.923076923076923</v>
       </c>
       <c r="D15" t="n">
-        <v>104</v>
+        <v>572</v>
       </c>
       <c r="E15" t="n">
-        <v>1.375</v>
+        <v>1.694055944055944</v>
       </c>
       <c r="F15" t="n">
-        <v>7229</v>
+        <v>34128</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>[('Saturday', 195), ('Friday', 96), ('Tuesday', 82)]</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>79.65909090909091</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>['English']</t>
+        </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>Portugal</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>January</t>
+          <t>March</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4</v>
+        <v>3.949392712550607</v>
       </c>
       <c r="D16" t="n">
-        <v>120</v>
+        <v>494</v>
       </c>
       <c r="E16" t="n">
-        <v>1.375</v>
+        <v>1.629554655870445</v>
       </c>
       <c r="F16" t="n">
-        <v>10215</v>
+        <v>33100.7</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>[('Friday', 106), ('Wednesday', 92), ('Monday', 71)]</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>95.16538461538461</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>['English']</t>
+        </is>
       </c>
     </row>
     <row r="17">
@@ -833,74 +1043,113 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>June</t>
+          <t>April</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>3.777777777777778</v>
+        <v>4.205128205128205</v>
       </c>
       <c r="D17" t="n">
-        <v>72</v>
+        <v>312</v>
       </c>
       <c r="E17" t="n">
         <v>1.375</v>
       </c>
       <c r="F17" t="n">
-        <v>5665</v>
+        <v>28415</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>[('Friday', 80), ('Sunday', 72), ('Saturday', 56)]</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>121.9487179487179</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>['English', 'German']</t>
+        </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>Greece</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>March</t>
+          <t>February</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>6</v>
+        <v>7.565749235474006</v>
       </c>
       <c r="D18" t="n">
-        <v>88</v>
+        <v>327</v>
       </c>
       <c r="E18" t="n">
-        <v>1.375</v>
+        <v>1.749235474006116</v>
       </c>
       <c r="F18" t="n">
-        <v>12595</v>
+        <v>26937</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>[('Saturday', 110), ('Friday', 68), ('Sunday', 63)]</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
+        <v>103.6697247706422</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>['English']</t>
+        </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>Portugal</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>May</t>
+          <t>November</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>5.272727272727272</v>
+        <v>4.085106382978723</v>
       </c>
       <c r="D19" t="n">
-        <v>88</v>
+        <v>329</v>
       </c>
       <c r="E19" t="n">
-        <v>1.375</v>
+        <v>1.288753799392097</v>
       </c>
       <c r="F19" t="n">
-        <v>10739</v>
+        <v>20496.6</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>[('Friday', 66), ('Wednesday', 59), ('Saturday', 50)]</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>84.58237082066869</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>['English']</t>
+        </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -909,40 +1158,66 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>4.557692307692307</v>
+        <v>4.212355212355212</v>
       </c>
       <c r="D20" t="n">
-        <v>52</v>
+        <v>259</v>
       </c>
       <c r="E20" t="n">
-        <v>1.288461538461539</v>
+        <v>1.173745173745174</v>
       </c>
       <c r="F20" t="n">
-        <v>4614</v>
+        <v>19154.92</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>[('Friday', 75), ('Thursday', 54), ('Monday', 41)]</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
+        <v>97.1888030888031</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>['French']</t>
+        </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>October</t>
+          <t>August</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>3.844660194174757</v>
+        <v>4.133928571428571</v>
       </c>
       <c r="D21" t="n">
-        <v>206</v>
+        <v>224</v>
       </c>
       <c r="E21" t="n">
-        <v>1.276699029126214</v>
+        <v>1.209821428571429</v>
       </c>
       <c r="F21" t="n">
-        <v>13953</v>
+        <v>18747.7</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>[('Saturday', 40), ('Sunday', 40), ('Friday', 34)]</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>111.1859821428571</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>['English']</t>
+        </is>
       </c>
     </row>
     <row r="22">
@@ -953,92 +1228,144 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>September</t>
+          <t>October</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>3.75</v>
+        <v>3.844660194174757</v>
       </c>
       <c r="D22" t="n">
-        <v>64</v>
+        <v>206</v>
       </c>
       <c r="E22" t="n">
-        <v>1.375</v>
+        <v>1.276699029126214</v>
       </c>
       <c r="F22" t="n">
-        <v>4161.12</v>
+        <v>13953</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>[('Sunday', 57), ('Wednesday', 43), ('Tuesday', 37)]</t>
+        </is>
+      </c>
+      <c r="H22" t="n">
+        <v>94.75728155339806</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>['German']</t>
+        </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Portugal</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>April</t>
+          <t>September</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>4.089038385437277</v>
+        <v>3.989690721649485</v>
       </c>
       <c r="D23" t="n">
-        <v>2527</v>
+        <v>194</v>
       </c>
       <c r="E23" t="n">
-        <v>1.6398891966759</v>
+        <v>1.164948453608248</v>
       </c>
       <c r="F23" t="n">
-        <v>173967.5</v>
+        <v>13759.46</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>[('Saturday', 44), ('Wednesday', 38), ('Friday', 36)]</t>
+        </is>
+      </c>
+      <c r="H23" t="n">
+        <v>97.52226804123711</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>['English']</t>
+        </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Portugal</t>
+          <t>Greece</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>August</t>
+          <t>November</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>4.164769647696477</v>
+        <v>4.117021276595745</v>
       </c>
       <c r="D24" t="n">
-        <v>1845</v>
+        <v>282</v>
       </c>
       <c r="E24" t="n">
-        <v>1.38319783197832</v>
+        <v>1.439716312056738</v>
       </c>
       <c r="F24" t="n">
-        <v>119299.68</v>
+        <v>12941.32</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>[('Friday', 73), ('Saturday', 60), ('Thursday', 54)]</t>
+        </is>
+      </c>
+      <c r="H24" t="n">
+        <v>61.03460992907801</v>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>['Spanish']</t>
+        </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Portugal</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>December</t>
+          <t>March</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>4.112244897959184</v>
+        <v>6</v>
       </c>
       <c r="D25" t="n">
-        <v>196</v>
+        <v>88</v>
       </c>
       <c r="E25" t="n">
-        <v>1.173469387755102</v>
+        <v>1.375</v>
       </c>
       <c r="F25" t="n">
-        <v>10991.2</v>
+        <v>12595</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>[('Tuesday', 32), ('Wednesday', 16), ('Saturday', 16)]</t>
+        </is>
+      </c>
+      <c r="H25" t="n">
+        <v>174</v>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>['German']</t>
+        </is>
       </c>
     </row>
     <row r="26">
@@ -1049,44 +1376,70 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>February</t>
+          <t>December</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>3.720812182741117</v>
+        <v>4.112244897959184</v>
       </c>
       <c r="D26" t="n">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E26" t="n">
-        <v>1.467005076142132</v>
+        <v>1.173469387755102</v>
       </c>
       <c r="F26" t="n">
-        <v>10560.04</v>
+        <v>10991.2</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>[('Friday', 80), ('Saturday', 48), ('Sunday', 21)]</t>
+        </is>
+      </c>
+      <c r="H26" t="n">
+        <v>75.80714285714286</v>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>['Spanish']</t>
+        </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Portugal</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>January</t>
+          <t>May</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>3.961832061068702</v>
+        <v>5.272727272727272</v>
       </c>
       <c r="D27" t="n">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="E27" t="n">
-        <v>1.595419847328244</v>
+        <v>1.375</v>
       </c>
       <c r="F27" t="n">
-        <v>7772</v>
+        <v>10739</v>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>[('Wednesday', 40), ('Thursday', 16), ('Saturday', 16)]</t>
+        </is>
+      </c>
+      <c r="H27" t="n">
+        <v>152.9090909090909</v>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>['English', 'German']</t>
+        </is>
       </c>
     </row>
     <row r="28">
@@ -1097,44 +1450,70 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>June</t>
+          <t>February</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>4.231991525423729</v>
+        <v>3.720812182741117</v>
       </c>
       <c r="D28" t="n">
-        <v>1888</v>
+        <v>197</v>
       </c>
       <c r="E28" t="n">
-        <v>1.621822033898305</v>
+        <v>1.467005076142132</v>
       </c>
       <c r="F28" t="n">
-        <v>136740.7</v>
+        <v>10560.04</v>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>[('Saturday', 47), ('Monday', 35), ('Wednesday', 26)]</t>
+        </is>
+      </c>
+      <c r="H28" t="n">
+        <v>79.57888324873097</v>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>['English']</t>
+        </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Portugal</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>March</t>
+          <t>January</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>3.949392712550607</v>
+        <v>4</v>
       </c>
       <c r="D29" t="n">
-        <v>494</v>
+        <v>120</v>
       </c>
       <c r="E29" t="n">
-        <v>1.629554655870445</v>
+        <v>1.375</v>
       </c>
       <c r="F29" t="n">
-        <v>33100.7</v>
+        <v>10215</v>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>[('Wednesday', 40), ('Thursday', 40), ('Sunday', 16)]</t>
+        </is>
+      </c>
+      <c r="H29" t="n">
+        <v>116</v>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>['Italian']</t>
+        </is>
       </c>
     </row>
     <row r="30">
@@ -1145,92 +1524,144 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>May</t>
+          <t>January</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>4.262116316639742</v>
+        <v>3.961832061068702</v>
       </c>
       <c r="D30" t="n">
-        <v>2476</v>
+        <v>131</v>
       </c>
       <c r="E30" t="n">
-        <v>1.644184168012924</v>
+        <v>1.595419847328244</v>
       </c>
       <c r="F30" t="n">
-        <v>179698</v>
+        <v>7772</v>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>[('Wednesday', 43), ('Monday', 31), ('Friday', 18)]</t>
+        </is>
+      </c>
+      <c r="H30" t="n">
+        <v>86.19083969465649</v>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>['English']</t>
+        </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Portugal</t>
+          <t>Greece</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>November</t>
+          <t>January</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>4.085106382978723</v>
+        <v>4.215568862275449</v>
       </c>
       <c r="D31" t="n">
-        <v>329</v>
+        <v>167</v>
       </c>
       <c r="E31" t="n">
-        <v>1.288753799392097</v>
+        <v>1.491017964071856</v>
       </c>
       <c r="F31" t="n">
-        <v>20496.6</v>
+        <v>7348.5</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>[('Friday', 56), ('Saturday', 35), ('Tuesday', 28)]</t>
+        </is>
+      </c>
+      <c r="H31" t="n">
+        <v>62.77844311377245</v>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>['English']</t>
+        </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Portugal</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>October</t>
+          <t>April</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>3.954545454545455</v>
+        <v>4.551724137931035</v>
       </c>
       <c r="D32" t="n">
-        <v>1100</v>
+        <v>87</v>
       </c>
       <c r="E32" t="n">
-        <v>1.493636363636364</v>
+        <v>1.172413793103448</v>
       </c>
       <c r="F32" t="n">
-        <v>70794.60000000001</v>
+        <v>7231.46</v>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>[('Thursday', 26), ('Sunday', 25), ('Saturday', 13)]</t>
+        </is>
+      </c>
+      <c r="H32" t="n">
+        <v>109.1075862068966</v>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>['English']</t>
+        </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Portugal</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>September</t>
+          <t>February</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>3.888774459320288</v>
+        <v>3.461538461538462</v>
       </c>
       <c r="D33" t="n">
-        <v>971</v>
+        <v>104</v>
       </c>
       <c r="E33" t="n">
-        <v>1.440782698249228</v>
+        <v>1.375</v>
       </c>
       <c r="F33" t="n">
-        <v>58716</v>
+        <v>7229</v>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>[('Saturday', 32), ('Friday', 32), ('Tuesday', 16)]</t>
+        </is>
+      </c>
+      <c r="H33" t="n">
+        <v>100.3846153846154</v>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>['English']</t>
+        </is>
       </c>
     </row>
     <row r="34">
@@ -1241,44 +1672,70 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>April</t>
+          <t>May</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>4.551724137931035</v>
+        <v>3.777777777777778</v>
       </c>
       <c r="D34" t="n">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E34" t="n">
-        <v>1.172413793103448</v>
+        <v>1.209876543209877</v>
       </c>
       <c r="F34" t="n">
-        <v>7231.46</v>
+        <v>5793.78</v>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>[('Sunday', 22), ('Monday', 22), ('Thursday', 17)]</t>
+        </is>
+      </c>
+      <c r="H34" t="n">
+        <v>97.99654320987655</v>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>['English']</t>
+        </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>August</t>
+          <t>June</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>4.133928571428571</v>
+        <v>3.777777777777778</v>
       </c>
       <c r="D35" t="n">
-        <v>224</v>
+        <v>72</v>
       </c>
       <c r="E35" t="n">
-        <v>1.209821428571429</v>
+        <v>1.375</v>
       </c>
       <c r="F35" t="n">
-        <v>18747.7</v>
+        <v>5665</v>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>[('Tuesday', 24), ('Friday', 24), ('Thursday', 16)]</t>
+        </is>
+      </c>
+      <c r="H35" t="n">
+        <v>109.5555555555556</v>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>['English']</t>
+        </is>
       </c>
     </row>
     <row r="36">
@@ -1289,68 +1746,107 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>December</t>
+          <t>June</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>3.777777777777778</v>
+        <v>3.567901234567901</v>
       </c>
       <c r="D36" t="n">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="E36" t="n">
-        <v>1.155555555555555</v>
+        <v>1.185185185185185</v>
       </c>
       <c r="F36" t="n">
-        <v>2890</v>
+        <v>5520.82</v>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>[('Thursday', 20), ('Tuesday', 15), ('Monday', 10)]</t>
+        </is>
+      </c>
+      <c r="H36" t="n">
+        <v>95.15753086419754</v>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>['English']</t>
+        </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>June</t>
+          <t>November</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>3.567901234567901</v>
+        <v>4.557692307692307</v>
       </c>
       <c r="D37" t="n">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="E37" t="n">
-        <v>1.185185185185185</v>
+        <v>1.288461538461539</v>
       </c>
       <c r="F37" t="n">
-        <v>5520.82</v>
+        <v>4614</v>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>[('Thursday', 25), ('Wednesday', 11), ('Friday', 8)]</t>
+        </is>
+      </c>
+      <c r="H37" t="n">
+        <v>115.4038461538462</v>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>['English']</t>
+        </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>May</t>
+          <t>September</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>3.777777777777778</v>
+        <v>3.75</v>
       </c>
       <c r="D38" t="n">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="E38" t="n">
-        <v>1.209876543209877</v>
+        <v>1.375</v>
       </c>
       <c r="F38" t="n">
-        <v>5793.78</v>
+        <v>4161.12</v>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>[('Tuesday', 24), ('Friday', 16), ('Wednesday', 8)]</t>
+        </is>
+      </c>
+      <c r="H38" t="n">
+        <v>95.8925</v>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>['Spanish']</t>
+        </is>
       </c>
     </row>
     <row r="39">
@@ -1361,92 +1857,144 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>November</t>
+          <t>December</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>4.212355212355212</v>
+        <v>3.777777777777778</v>
       </c>
       <c r="D39" t="n">
-        <v>259</v>
+        <v>45</v>
       </c>
       <c r="E39" t="n">
-        <v>1.173745173745174</v>
+        <v>1.155555555555555</v>
       </c>
       <c r="F39" t="n">
-        <v>19154.92</v>
+        <v>2890</v>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>[('Saturday', 11), ('Thursday', 10), ('Friday', 8)]</t>
+        </is>
+      </c>
+      <c r="H39" t="n">
+        <v>87.73333333333333</v>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>['Spanish']</t>
+        </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>October</t>
+          <t>September</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>3.787446504992867</v>
+        <v>2.64</v>
       </c>
       <c r="D40" t="n">
-        <v>701</v>
+        <v>50</v>
       </c>
       <c r="E40" t="n">
-        <v>1.156918687589158</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
-        <v>47079.84</v>
+        <v>2710</v>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>[('Tuesday', 14), ('Sunday', 10), ('Wednesday', 8)]</t>
+        </is>
+      </c>
+      <c r="H40" t="n">
+        <v>90.2</v>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>['English']</t>
+        </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>September</t>
+          <t>August</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>3.989690721649485</v>
+        <v>3</v>
       </c>
       <c r="D41" t="n">
-        <v>194</v>
+        <v>40</v>
       </c>
       <c r="E41" t="n">
-        <v>1.164948453608248</v>
+        <v>1.375</v>
       </c>
       <c r="F41" t="n">
-        <v>13759.46</v>
+        <v>2245</v>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>[('Sunday', 16), ('Wednesday', 8), ('Thursday', 8)]</t>
+        </is>
+      </c>
+      <c r="H41" t="n">
+        <v>87</v>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>['German']</t>
+        </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Greece</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>October</t>
+          <t>December</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>2.311111111111111</v>
+        <v>4.520833333333333</v>
       </c>
       <c r="D42" t="n">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>1.208333333333333</v>
       </c>
       <c r="F42" t="n">
-        <v>2038</v>
+        <v>2150.8</v>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>[('Saturday', 22), ('Thursday', 10), ('Wednesday', 5)]</t>
+        </is>
+      </c>
+      <c r="H42" t="n">
+        <v>59.01666666666667</v>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>['Spanish']</t>
+        </is>
       </c>
     </row>
     <row r="43">
@@ -1457,20 +2005,33 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>September</t>
+          <t>October</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>2.64</v>
+        <v>2.311111111111111</v>
       </c>
       <c r="D43" t="n">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E43" t="n">
         <v>1</v>
       </c>
       <c r="F43" t="n">
-        <v>2710</v>
+        <v>2038</v>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>[('Sunday', 10), ('Wednesday', 10), ('Monday', 10)]</t>
+        </is>
+      </c>
+      <c r="H43" t="n">
+        <v>80.88888888888889</v>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>['English']</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added average spending per travellers
</commit_message>
<xml_diff>
--- a/questions/successful_tour_looks_like.xlsx
+++ b/questions/successful_tour_looks_like.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,6 +479,11 @@
           <t>most_common_languages</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>most_common_number_of_stories</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -516,6 +521,9 @@
           <t>['English']</t>
         </is>
       </c>
+      <c r="J2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -553,6 +561,9 @@
           <t>['English']</t>
         </is>
       </c>
+      <c r="J3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -590,6 +601,9 @@
           <t>['English']</t>
         </is>
       </c>
+      <c r="J4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -627,6 +641,9 @@
           <t>['English']</t>
         </is>
       </c>
+      <c r="J5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -664,6 +681,9 @@
           <t>['English']</t>
         </is>
       </c>
+      <c r="J6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -701,6 +721,9 @@
           <t>['English']</t>
         </is>
       </c>
+      <c r="J7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -738,6 +761,9 @@
           <t>['English']</t>
         </is>
       </c>
+      <c r="J8" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -775,6 +801,9 @@
           <t>['English']</t>
         </is>
       </c>
+      <c r="J9" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -812,6 +841,9 @@
           <t>['English']</t>
         </is>
       </c>
+      <c r="J10" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -849,6 +881,9 @@
           <t>['English']</t>
         </is>
       </c>
+      <c r="J11" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -886,6 +921,9 @@
           <t>['English']</t>
         </is>
       </c>
+      <c r="J12" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -923,6 +961,9 @@
           <t>['English']</t>
         </is>
       </c>
+      <c r="J13" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -960,6 +1001,9 @@
           <t>['English']</t>
         </is>
       </c>
+      <c r="J14" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -997,6 +1041,9 @@
           <t>['English']</t>
         </is>
       </c>
+      <c r="J15" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1034,6 +1081,9 @@
           <t>['English']</t>
         </is>
       </c>
+      <c r="J16" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1071,6 +1121,9 @@
           <t>['English', 'German']</t>
         </is>
       </c>
+      <c r="J17" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1108,6 +1161,9 @@
           <t>['English']</t>
         </is>
       </c>
+      <c r="J18" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1145,6 +1201,9 @@
           <t>['English']</t>
         </is>
       </c>
+      <c r="J19" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1182,6 +1241,9 @@
           <t>['French']</t>
         </is>
       </c>
+      <c r="J20" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1219,6 +1281,9 @@
           <t>['English']</t>
         </is>
       </c>
+      <c r="J21" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1256,6 +1321,9 @@
           <t>['German']</t>
         </is>
       </c>
+      <c r="J22" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1293,6 +1361,9 @@
           <t>['English']</t>
         </is>
       </c>
+      <c r="J23" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1330,6 +1401,9 @@
           <t>['Spanish']</t>
         </is>
       </c>
+      <c r="J24" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1367,6 +1441,9 @@
           <t>['German']</t>
         </is>
       </c>
+      <c r="J25" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1404,6 +1481,9 @@
           <t>['Spanish']</t>
         </is>
       </c>
+      <c r="J26" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1441,6 +1521,9 @@
           <t>['English', 'German']</t>
         </is>
       </c>
+      <c r="J27" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1478,6 +1561,9 @@
           <t>['English']</t>
         </is>
       </c>
+      <c r="J28" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1515,6 +1601,9 @@
           <t>['Italian']</t>
         </is>
       </c>
+      <c r="J29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1552,6 +1641,9 @@
           <t>['English']</t>
         </is>
       </c>
+      <c r="J30" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1589,6 +1681,9 @@
           <t>['English']</t>
         </is>
       </c>
+      <c r="J31" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1626,6 +1721,9 @@
           <t>['English']</t>
         </is>
       </c>
+      <c r="J32" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1663,6 +1761,9 @@
           <t>['English']</t>
         </is>
       </c>
+      <c r="J33" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1700,6 +1801,9 @@
           <t>['English']</t>
         </is>
       </c>
+      <c r="J34" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1737,6 +1841,9 @@
           <t>['English']</t>
         </is>
       </c>
+      <c r="J35" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1774,6 +1881,9 @@
           <t>['English']</t>
         </is>
       </c>
+      <c r="J36" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1811,6 +1921,9 @@
           <t>['English']</t>
         </is>
       </c>
+      <c r="J37" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1848,6 +1961,9 @@
           <t>['Spanish']</t>
         </is>
       </c>
+      <c r="J38" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1885,6 +2001,9 @@
           <t>['Spanish']</t>
         </is>
       </c>
+      <c r="J39" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1922,6 +2041,9 @@
           <t>['English']</t>
         </is>
       </c>
+      <c r="J40" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1959,6 +2081,9 @@
           <t>['German']</t>
         </is>
       </c>
+      <c r="J41" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1996,6 +2121,9 @@
           <t>['Spanish']</t>
         </is>
       </c>
+      <c r="J42" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2032,6 +2160,9 @@
         <is>
           <t>['English']</t>
         </is>
+      </c>
+      <c r="J43" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>